<commit_message>
remplaza por copias identicas a las halladas en el repo del app
</commit_message>
<xml_diff>
--- a/DataBases/ENCoR/DICCIONARIO DE VARIABLES.xlsx
+++ b/DataBases/ENCoR/DICCIONARIO DE VARIABLES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dacza\Dropbox\UnaImagen\DataBases\ENCoR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dacza\Dropbox\UnaImagen - Apps\AppENCoR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1614,7 +1614,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1641,12 +1641,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1659,13 +1653,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,7 +1884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1919,9 +1961,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1955,6 +1994,207 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1964,6 +2204,135 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1976,254 +2345,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2536,38 +2659,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
-      <selection activeCell="A376" sqref="A376"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="86" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" style="37" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="36" customWidth="1"/>
     <col min="3" max="3" width="56.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="134" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="135"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
+      <c r="A2" s="136"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="137"/>
     </row>
     <row r="3" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>308</v>
       </c>
     </row>
@@ -2575,7 +2698,7 @@
       <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="25" t="s">
         <v>2</v>
       </c>
@@ -2584,7 +2707,7 @@
       <c r="A5" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>140</v>
       </c>
       <c r="C5" s="3"/>
@@ -2593,25 +2716,25 @@
       <c r="A6" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>139</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="93" t="s">
         <v>160</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>160</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="94" t="s">
         <v>310</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>161</v>
       </c>
       <c r="C8" s="21"/>
@@ -2620,16 +2743,16 @@
       <c r="A9" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>162</v>
       </c>
       <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="104" t="s">
         <v>312</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>163</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -2637,24 +2760,24 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="150" t="s">
         <v>313</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>164</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -2662,8 +2785,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="151"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="10" t="s">
         <v>11</v>
       </c>
@@ -2672,7 +2795,7 @@
       <c r="A15" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>166</v>
       </c>
       <c r="C15" s="21"/>
@@ -2681,7 +2804,7 @@
       <c r="A16" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>165</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -2690,35 +2813,35 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
-      <c r="B17" s="33"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
-      <c r="B18" s="33"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
-      <c r="B19" s="33"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
-      <c r="B20" s="33"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
-      <c r="B21" s="35"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="13" t="s">
         <v>17</v>
       </c>
@@ -2727,14 +2850,14 @@
       <c r="A22" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="31"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="25"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>167</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -2743,16 +2866,16 @@
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="23"/>
-      <c r="B24" s="35"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="141" t="s">
         <v>317</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="32" t="s">
         <v>168</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -2760,8 +2883,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="142"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="13" t="s">
         <v>11</v>
       </c>
@@ -2770,7 +2893,7 @@
       <c r="A27" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>169</v>
       </c>
       <c r="C27" s="21"/>
@@ -2779,7 +2902,7 @@
       <c r="A28" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>170</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -2788,91 +2911,91 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
-      <c r="B29" s="33"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
-      <c r="B30" s="33"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
-      <c r="B31" s="33"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
-      <c r="B32" s="33"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
-      <c r="B33" s="33"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
-      <c r="B34" s="33"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
-      <c r="B35" s="33"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
-      <c r="B36" s="33"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
-      <c r="B37" s="33"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
-      <c r="B38" s="33"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
-      <c r="B39" s="33"/>
+      <c r="B39" s="32"/>
       <c r="C39" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
-      <c r="B40" s="33"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11"/>
-      <c r="B41" s="35"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="13" t="s">
         <v>32</v>
       </c>
@@ -2881,14 +3004,14 @@
       <c r="A42" s="22" t="s">
         <v>446</v>
       </c>
-      <c r="B42" s="31"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="25"/>
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="113" t="s">
         <v>320</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="33" t="s">
         <v>171</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -2896,8 +3019,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="56"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="143"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="13" t="s">
         <v>34</v>
       </c>
@@ -2906,7 +3029,7 @@
       <c r="A45" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="31" t="s">
         <v>172</v>
       </c>
       <c r="C45" s="21"/>
@@ -2915,7 +3038,7 @@
       <c r="A46" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="33" t="s">
         <v>173</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -2924,7 +3047,7 @@
     </row>
     <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11"/>
-      <c r="B47" s="35"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="13" t="s">
         <v>34</v>
       </c>
@@ -2933,7 +3056,7 @@
       <c r="A48" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C48" s="21"/>
@@ -2942,7 +3065,7 @@
       <c r="A49" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="138" t="s">
         <v>175</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -2951,49 +3074,49 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
-      <c r="B50" s="53"/>
+      <c r="B50" s="139"/>
       <c r="C50" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
-      <c r="B51" s="53"/>
+      <c r="B51" s="139"/>
       <c r="C51" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
-      <c r="B52" s="53"/>
+      <c r="B52" s="139"/>
       <c r="C52" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
-      <c r="B53" s="53"/>
+      <c r="B53" s="139"/>
       <c r="C53" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
-      <c r="B54" s="53"/>
+      <c r="B54" s="139"/>
       <c r="C54" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
-      <c r="B55" s="53"/>
+      <c r="B55" s="139"/>
       <c r="C55" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11"/>
-      <c r="B56" s="54"/>
+      <c r="B56" s="140"/>
       <c r="C56" s="13" t="s">
         <v>32</v>
       </c>
@@ -3002,7 +3125,7 @@
       <c r="A57" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -3011,84 +3134,84 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
-      <c r="B58" s="33"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
-      <c r="B59" s="33"/>
+      <c r="B59" s="32"/>
       <c r="C59" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
-      <c r="B60" s="33"/>
+      <c r="B60" s="32"/>
       <c r="C60" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
-      <c r="B61" s="33"/>
+      <c r="B61" s="32"/>
       <c r="C61" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
-      <c r="B62" s="33"/>
+      <c r="B62" s="32"/>
       <c r="C62" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
-      <c r="B63" s="33"/>
+      <c r="B63" s="32"/>
       <c r="C63" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
-      <c r="B64" s="33"/>
+      <c r="B64" s="32"/>
       <c r="C64" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
-      <c r="B65" s="33"/>
+      <c r="B65" s="32"/>
       <c r="C65" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
-      <c r="B66" s="33"/>
+      <c r="B66" s="32"/>
       <c r="C66" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
-      <c r="B67" s="33"/>
+      <c r="B67" s="32"/>
       <c r="C67" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
-      <c r="B68" s="33"/>
+      <c r="B68" s="32"/>
       <c r="C68" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11"/>
-      <c r="B69" s="35"/>
+      <c r="B69" s="34"/>
       <c r="C69" s="13" t="s">
         <v>52</v>
       </c>
@@ -3097,7 +3220,7 @@
       <c r="A70" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B70" s="34" t="s">
+      <c r="B70" s="33" t="s">
         <v>177</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -3106,14 +3229,14 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
-      <c r="B71" s="33"/>
+      <c r="B71" s="32"/>
       <c r="C71" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="11"/>
-      <c r="B72" s="35"/>
+      <c r="B72" s="34"/>
       <c r="C72" s="13" t="s">
         <v>55</v>
       </c>
@@ -3122,14 +3245,14 @@
       <c r="A73" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="36"/>
+      <c r="B73" s="35"/>
       <c r="C73" s="25"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="33" t="s">
         <v>141</v>
       </c>
       <c r="C74" s="7" t="s">
@@ -3138,7 +3261,7 @@
     </row>
     <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11"/>
-      <c r="B75" s="35"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="12" t="s">
         <v>54</v>
       </c>
@@ -3147,7 +3270,7 @@
       <c r="A76" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="B76" s="32" t="s">
+      <c r="B76" s="31" t="s">
         <v>142</v>
       </c>
       <c r="C76" s="2"/>
@@ -3156,7 +3279,7 @@
       <c r="A77" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="B77" s="32" t="s">
+      <c r="B77" s="31" t="s">
         <v>306</v>
       </c>
       <c r="C77" s="16"/>
@@ -3165,14 +3288,14 @@
       <c r="A78" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="B78" s="32" t="s">
+      <c r="B78" s="31" t="s">
         <v>159</v>
       </c>
       <c r="C78" s="16"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="17"/>
-      <c r="B79" s="52" t="s">
+      <c r="B79" s="138" t="s">
         <v>459</v>
       </c>
       <c r="C79" s="18" t="s">
@@ -3183,7 +3306,7 @@
       <c r="A80" s="17" t="s">
         <v>460</v>
       </c>
-      <c r="B80" s="54"/>
+      <c r="B80" s="140"/>
       <c r="C80" s="19" t="s">
         <v>462</v>
       </c>
@@ -3192,7 +3315,7 @@
       <c r="A81" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B81" s="34" t="s">
+      <c r="B81" s="33" t="s">
         <v>143</v>
       </c>
       <c r="C81" s="8" t="s">
@@ -3201,7 +3324,7 @@
     </row>
     <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11"/>
-      <c r="B82" s="35"/>
+      <c r="B82" s="34"/>
       <c r="C82" s="13" t="s">
         <v>57</v>
       </c>
@@ -3210,7 +3333,7 @@
       <c r="A83" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="B83" s="34" t="s">
+      <c r="B83" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C83" s="8" t="s">
@@ -3219,21 +3342,21 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="9"/>
-      <c r="B84" s="33"/>
+      <c r="B84" s="32"/>
       <c r="C84" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
-      <c r="B85" s="33"/>
+      <c r="B85" s="32"/>
       <c r="C85" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="11"/>
-      <c r="B86" s="35"/>
+      <c r="B86" s="34"/>
       <c r="C86" s="13" t="s">
         <v>65</v>
       </c>
@@ -3242,7 +3365,7 @@
       <c r="A87" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B87" s="34" t="s">
+      <c r="B87" s="33" t="s">
         <v>145</v>
       </c>
       <c r="C87" s="8" t="s">
@@ -3251,14 +3374,14 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="9"/>
-      <c r="B88" s="33"/>
+      <c r="B88" s="32"/>
       <c r="C88" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11"/>
-      <c r="B89" s="35"/>
+      <c r="B89" s="34"/>
       <c r="C89" s="13" t="s">
         <v>62</v>
       </c>
@@ -3267,7 +3390,7 @@
       <c r="A90" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="B90" s="34" t="s">
+      <c r="B90" s="33" t="s">
         <v>146</v>
       </c>
       <c r="C90" s="7" t="s">
@@ -3276,7 +3399,7 @@
     </row>
     <row r="91" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
-      <c r="B91" s="33"/>
+      <c r="B91" s="32"/>
       <c r="C91" s="4" t="s">
         <v>54</v>
       </c>
@@ -3285,7 +3408,7 @@
       <c r="A92" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B92" s="34" t="s">
+      <c r="B92" s="33" t="s">
         <v>147</v>
       </c>
       <c r="C92" s="7" t="s">
@@ -3294,14 +3417,14 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
-      <c r="B93" s="33"/>
+      <c r="B93" s="32"/>
       <c r="C93" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="11"/>
-      <c r="B94" s="35"/>
+      <c r="B94" s="34"/>
       <c r="C94" s="12" t="s">
         <v>66</v>
       </c>
@@ -3310,7 +3433,7 @@
       <c r="A95" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="B95" s="34" t="s">
+      <c r="B95" s="33" t="s">
         <v>148</v>
       </c>
       <c r="C95" s="7" t="s">
@@ -3319,14 +3442,14 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="9"/>
-      <c r="B96" s="33"/>
+      <c r="B96" s="32"/>
       <c r="C96" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="11"/>
-      <c r="B97" s="35"/>
+      <c r="B97" s="34"/>
       <c r="C97" s="12" t="s">
         <v>68</v>
       </c>
@@ -3335,7 +3458,7 @@
       <c r="A98" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="B98" s="34" t="s">
+      <c r="B98" s="33" t="s">
         <v>149</v>
       </c>
       <c r="C98" s="7" t="s">
@@ -3344,16 +3467,16 @@
     </row>
     <row r="99" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
-      <c r="B99" s="33"/>
+      <c r="B99" s="32"/>
       <c r="C99" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="55" t="s">
+      <c r="A100" s="113" t="s">
         <v>338</v>
       </c>
-      <c r="B100" s="34" t="s">
+      <c r="B100" s="33" t="s">
         <v>150</v>
       </c>
       <c r="C100" s="8" t="s">
@@ -3361,15 +3484,15 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="60"/>
-      <c r="B101" s="33"/>
+      <c r="A101" s="114"/>
+      <c r="B101" s="32"/>
       <c r="C101" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="20"/>
-      <c r="B102" s="35"/>
+      <c r="B102" s="34"/>
       <c r="C102" s="13" t="s">
         <v>69</v>
       </c>
@@ -3378,7 +3501,7 @@
       <c r="A103" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="B103" s="34" t="s">
+      <c r="B103" s="33" t="s">
         <v>151</v>
       </c>
       <c r="C103" s="8" t="s">
@@ -3387,7 +3510,7 @@
     </row>
     <row r="104" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="11"/>
-      <c r="B104" s="35"/>
+      <c r="B104" s="34"/>
       <c r="C104" s="13" t="s">
         <v>54</v>
       </c>
@@ -3396,7 +3519,7 @@
       <c r="A105" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="B105" s="34" t="s">
+      <c r="B105" s="33" t="s">
         <v>152</v>
       </c>
       <c r="C105" s="8" t="s">
@@ -3405,7 +3528,7 @@
     </row>
     <row r="106" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="11"/>
-      <c r="B106" s="35"/>
+      <c r="B106" s="34"/>
       <c r="C106" s="13" t="s">
         <v>71</v>
       </c>
@@ -3414,7 +3537,7 @@
       <c r="A107" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="B107" s="32" t="s">
+      <c r="B107" s="31" t="s">
         <v>153</v>
       </c>
       <c r="C107" s="21"/>
@@ -3423,7 +3546,7 @@
       <c r="A108" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="B108" s="34" t="s">
+      <c r="B108" s="33" t="s">
         <v>154</v>
       </c>
       <c r="C108" s="8" t="s">
@@ -3432,16 +3555,16 @@
     </row>
     <row r="109" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="11"/>
-      <c r="B109" s="35"/>
+      <c r="B109" s="34"/>
       <c r="C109" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="61" t="s">
+      <c r="A110" s="119" t="s">
         <v>343</v>
       </c>
-      <c r="B110" s="34" t="s">
+      <c r="B110" s="33" t="s">
         <v>155</v>
       </c>
       <c r="C110" s="8" t="s">
@@ -3449,15 +3572,15 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="62"/>
-      <c r="B111" s="33"/>
+      <c r="A111" s="120"/>
+      <c r="B111" s="32"/>
       <c r="C111" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="63"/>
-      <c r="B112" s="35"/>
+      <c r="A112" s="121"/>
+      <c r="B112" s="34"/>
       <c r="C112" s="13" t="s">
         <v>74</v>
       </c>
@@ -3466,7 +3589,7 @@
       <c r="A113" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B113" s="32" t="s">
+      <c r="B113" s="31" t="s">
         <v>156</v>
       </c>
       <c r="C113" s="13"/>
@@ -3475,7 +3598,7 @@
       <c r="A114" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="B114" s="32" t="s">
+      <c r="B114" s="31" t="s">
         <v>157</v>
       </c>
       <c r="C114" s="13"/>
@@ -3484,7 +3607,7 @@
       <c r="A115" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B115" s="32" t="s">
+      <c r="B115" s="31" t="s">
         <v>158</v>
       </c>
       <c r="C115" s="13"/>
@@ -3493,14 +3616,14 @@
       <c r="A116" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B116" s="31"/>
+      <c r="B116" s="30"/>
       <c r="C116" s="25"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B117" s="34" t="s">
+      <c r="B117" s="33" t="s">
         <v>237</v>
       </c>
       <c r="C117" s="8" t="s">
@@ -3509,14 +3632,14 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="9"/>
-      <c r="B118" s="33"/>
+      <c r="B118" s="32"/>
       <c r="C118" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="11"/>
-      <c r="B119" s="35"/>
+      <c r="B119" s="34"/>
       <c r="C119" s="13" t="s">
         <v>76</v>
       </c>
@@ -3525,7 +3648,7 @@
       <c r="A120" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="B120" s="34" t="s">
+      <c r="B120" s="33" t="s">
         <v>238</v>
       </c>
       <c r="C120" s="8" t="s">
@@ -3534,14 +3657,14 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="9"/>
-      <c r="B121" s="33"/>
+      <c r="B121" s="32"/>
       <c r="C121" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="11"/>
-      <c r="B122" s="35"/>
+      <c r="B122" s="34"/>
       <c r="C122" s="13" t="s">
         <v>60</v>
       </c>
@@ -3550,7 +3673,7 @@
       <c r="A123" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B123" s="34" t="s">
+      <c r="B123" s="33" t="s">
         <v>239</v>
       </c>
       <c r="C123" s="8" t="s">
@@ -3559,7 +3682,7 @@
     </row>
     <row r="124" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="11"/>
-      <c r="B124" s="35"/>
+      <c r="B124" s="34"/>
       <c r="C124" s="13" t="s">
         <v>54</v>
       </c>
@@ -3568,14 +3691,14 @@
       <c r="A125" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B125" s="36"/>
+      <c r="B125" s="35"/>
       <c r="C125" s="25"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="6" t="s">
+      <c r="A126" s="90" t="s">
         <v>347</v>
       </c>
-      <c r="B126" s="34" t="s">
+      <c r="B126" s="33" t="s">
         <v>240</v>
       </c>
       <c r="C126" s="8" t="s">
@@ -3583,17 +3706,17 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="11"/>
-      <c r="B127" s="35"/>
+      <c r="A127" s="91"/>
+      <c r="B127" s="34"/>
       <c r="C127" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="90" t="s">
         <v>348</v>
       </c>
-      <c r="B128" s="34" t="s">
+      <c r="B128" s="33" t="s">
         <v>241</v>
       </c>
       <c r="C128" s="8" t="s">
@@ -3601,26 +3724,26 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="11"/>
-      <c r="B129" s="35"/>
+      <c r="A129" s="91"/>
+      <c r="B129" s="34"/>
       <c r="C129" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="14" t="s">
+      <c r="A130" s="92" t="s">
         <v>349</v>
       </c>
-      <c r="B130" s="32" t="s">
+      <c r="B130" s="31" t="s">
         <v>242</v>
       </c>
       <c r="C130" s="21"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="B131" s="34" t="s">
+      <c r="B131" s="33" t="s">
         <v>243</v>
       </c>
       <c r="C131" s="8" t="s">
@@ -3628,17 +3751,17 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="11"/>
-      <c r="B132" s="35"/>
+      <c r="A132" s="96"/>
+      <c r="B132" s="34"/>
       <c r="C132" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="95" t="s">
         <v>351</v>
       </c>
-      <c r="B133" s="34" t="s">
+      <c r="B133" s="33" t="s">
         <v>244</v>
       </c>
       <c r="C133" s="8" t="s">
@@ -3646,17 +3769,17 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="11"/>
-      <c r="B134" s="35"/>
+      <c r="A134" s="96"/>
+      <c r="B134" s="34"/>
       <c r="C134" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="B135" s="34" t="s">
+      <c r="B135" s="33" t="s">
         <v>245</v>
       </c>
       <c r="C135" s="8" t="s">
@@ -3664,17 +3787,17 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="11"/>
-      <c r="B136" s="35"/>
+      <c r="A136" s="96"/>
+      <c r="B136" s="34"/>
       <c r="C136" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="9" t="s">
+      <c r="A137" s="97" t="s">
         <v>352</v>
       </c>
-      <c r="B137" s="33" t="s">
+      <c r="B137" s="32" t="s">
         <v>246</v>
       </c>
       <c r="C137" s="10" t="s">
@@ -3682,17 +3805,17 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="9"/>
-      <c r="B138" s="33"/>
+      <c r="A138" s="97"/>
+      <c r="B138" s="32"/>
       <c r="C138" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="6" t="s">
+      <c r="A139" s="95" t="s">
         <v>353</v>
       </c>
-      <c r="B139" s="34" t="s">
+      <c r="B139" s="33" t="s">
         <v>247</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -3700,17 +3823,17 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="11"/>
-      <c r="B140" s="35"/>
+      <c r="A140" s="96"/>
+      <c r="B140" s="34"/>
       <c r="C140" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="9" t="s">
+      <c r="A141" s="97" t="s">
         <v>354</v>
       </c>
-      <c r="B141" s="33" t="s">
+      <c r="B141" s="32" t="s">
         <v>248</v>
       </c>
       <c r="C141" s="10" t="s">
@@ -3718,17 +3841,17 @@
       </c>
     </row>
     <row r="142" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="9"/>
-      <c r="B142" s="33"/>
+      <c r="A142" s="97"/>
+      <c r="B142" s="32"/>
       <c r="C142" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="95" t="s">
         <v>355</v>
       </c>
-      <c r="B143" s="34" t="s">
+      <c r="B143" s="33" t="s">
         <v>249</v>
       </c>
       <c r="C143" s="8" t="s">
@@ -3736,17 +3859,17 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="11"/>
-      <c r="B144" s="35"/>
+      <c r="A144" s="96"/>
+      <c r="B144" s="34"/>
       <c r="C144" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="9" t="s">
+      <c r="A145" s="97" t="s">
         <v>356</v>
       </c>
-      <c r="B145" s="33" t="s">
+      <c r="B145" s="32" t="s">
         <v>250</v>
       </c>
       <c r="C145" s="8" t="s">
@@ -3754,17 +3877,17 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="9"/>
-      <c r="B146" s="33"/>
+      <c r="A146" s="97"/>
+      <c r="B146" s="32"/>
       <c r="C146" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="95" t="s">
         <v>357</v>
       </c>
-      <c r="B147" s="34" t="s">
+      <c r="B147" s="33" t="s">
         <v>251</v>
       </c>
       <c r="C147" s="8" t="s">
@@ -3772,17 +3895,17 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="11"/>
-      <c r="B148" s="35"/>
+      <c r="A148" s="96"/>
+      <c r="B148" s="34"/>
       <c r="C148" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="9" t="s">
+      <c r="A149" s="97" t="s">
         <v>358</v>
       </c>
-      <c r="B149" s="33" t="s">
+      <c r="B149" s="32" t="s">
         <v>252</v>
       </c>
       <c r="C149" s="8" t="s">
@@ -3790,17 +3913,17 @@
       </c>
     </row>
     <row r="150" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="9"/>
-      <c r="B150" s="33"/>
+      <c r="A150" s="97"/>
+      <c r="B150" s="32"/>
       <c r="C150" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="95" t="s">
         <v>359</v>
       </c>
-      <c r="B151" s="34" t="s">
+      <c r="B151" s="33" t="s">
         <v>253</v>
       </c>
       <c r="C151" s="8" t="s">
@@ -3808,17 +3931,17 @@
       </c>
     </row>
     <row r="152" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="11"/>
-      <c r="B152" s="35"/>
+      <c r="A152" s="96"/>
+      <c r="B152" s="34"/>
       <c r="C152" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="9" t="s">
+      <c r="A153" s="97" t="s">
         <v>360</v>
       </c>
-      <c r="B153" s="33" t="s">
+      <c r="B153" s="32" t="s">
         <v>254</v>
       </c>
       <c r="C153" s="8" t="s">
@@ -3826,17 +3949,17 @@
       </c>
     </row>
     <row r="154" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="9"/>
-      <c r="B154" s="33"/>
+      <c r="A154" s="97"/>
+      <c r="B154" s="32"/>
       <c r="C154" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="6" t="s">
+      <c r="A155" s="95" t="s">
         <v>361</v>
       </c>
-      <c r="B155" s="34" t="s">
+      <c r="B155" s="33" t="s">
         <v>255</v>
       </c>
       <c r="C155" s="8" t="s">
@@ -3844,17 +3967,17 @@
       </c>
     </row>
     <row r="156" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="11"/>
-      <c r="B156" s="35"/>
+      <c r="A156" s="96"/>
+      <c r="B156" s="34"/>
       <c r="C156" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="9" t="s">
+      <c r="A157" s="97" t="s">
         <v>362</v>
       </c>
-      <c r="B157" s="33" t="s">
+      <c r="B157" s="32" t="s">
         <v>256</v>
       </c>
       <c r="C157" s="8" t="s">
@@ -3862,17 +3985,17 @@
       </c>
     </row>
     <row r="158" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="9"/>
-      <c r="B158" s="33"/>
+      <c r="A158" s="97"/>
+      <c r="B158" s="32"/>
       <c r="C158" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="6" t="s">
+      <c r="A159" s="95" t="s">
         <v>363</v>
       </c>
-      <c r="B159" s="34" t="s">
+      <c r="B159" s="33" t="s">
         <v>257</v>
       </c>
       <c r="C159" s="8" t="s">
@@ -3880,17 +4003,17 @@
       </c>
     </row>
     <row r="160" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="11"/>
-      <c r="B160" s="35"/>
+      <c r="A160" s="96"/>
+      <c r="B160" s="34"/>
       <c r="C160" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="6" t="s">
+      <c r="A161" s="95" t="s">
         <v>364</v>
       </c>
-      <c r="B161" s="34" t="s">
+      <c r="B161" s="33" t="s">
         <v>258</v>
       </c>
       <c r="C161" s="8" t="s">
@@ -3898,17 +4021,17 @@
       </c>
     </row>
     <row r="162" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="11"/>
-      <c r="B162" s="35"/>
+      <c r="A162" s="96"/>
+      <c r="B162" s="34"/>
       <c r="C162" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="6" t="s">
+      <c r="A163" s="98" t="s">
         <v>365</v>
       </c>
-      <c r="B163" s="34" t="s">
+      <c r="B163" s="33" t="s">
         <v>259</v>
       </c>
       <c r="C163" s="8" t="s">
@@ -3916,17 +4039,17 @@
       </c>
     </row>
     <row r="164" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="11"/>
-      <c r="B164" s="35"/>
+      <c r="A164" s="99"/>
+      <c r="B164" s="34"/>
       <c r="C164" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="6" t="s">
+      <c r="A165" s="98" t="s">
         <v>366</v>
       </c>
-      <c r="B165" s="34" t="s">
+      <c r="B165" s="33" t="s">
         <v>260</v>
       </c>
       <c r="C165" s="8" t="s">
@@ -3934,17 +4057,17 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="11"/>
-      <c r="B166" s="35"/>
+      <c r="A166" s="99"/>
+      <c r="B166" s="34"/>
       <c r="C166" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="6" t="s">
+      <c r="A167" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="B167" s="34" t="s">
+      <c r="B167" s="33" t="s">
         <v>261</v>
       </c>
       <c r="C167" s="8" t="s">
@@ -3952,17 +4075,17 @@
       </c>
     </row>
     <row r="168" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="11"/>
-      <c r="B168" s="35"/>
+      <c r="A168" s="99"/>
+      <c r="B168" s="34"/>
       <c r="C168" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="9" t="s">
+      <c r="A169" s="100" t="s">
         <v>367</v>
       </c>
-      <c r="B169" s="33" t="s">
+      <c r="B169" s="32" t="s">
         <v>262</v>
       </c>
       <c r="C169" s="10" t="s">
@@ -3970,17 +4093,17 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="9"/>
-      <c r="B170" s="33"/>
+      <c r="A170" s="100"/>
+      <c r="B170" s="32"/>
       <c r="C170" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" s="6" t="s">
+      <c r="A171" s="98" t="s">
         <v>368</v>
       </c>
-      <c r="B171" s="34" t="s">
+      <c r="B171" s="33" t="s">
         <v>263</v>
       </c>
       <c r="C171" s="8" t="s">
@@ -3988,17 +4111,17 @@
       </c>
     </row>
     <row r="172" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="11"/>
-      <c r="B172" s="35"/>
+      <c r="A172" s="99"/>
+      <c r="B172" s="34"/>
       <c r="C172" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" s="9" t="s">
+      <c r="A173" s="100" t="s">
         <v>369</v>
       </c>
-      <c r="B173" s="33" t="s">
+      <c r="B173" s="32" t="s">
         <v>264</v>
       </c>
       <c r="C173" s="10" t="s">
@@ -4006,17 +4129,17 @@
       </c>
     </row>
     <row r="174" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="9"/>
-      <c r="B174" s="33"/>
+      <c r="A174" s="100"/>
+      <c r="B174" s="32"/>
       <c r="C174" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="6" t="s">
+      <c r="A175" s="98" t="s">
         <v>370</v>
       </c>
-      <c r="B175" s="34" t="s">
+      <c r="B175" s="33" t="s">
         <v>265</v>
       </c>
       <c r="C175" s="8" t="s">
@@ -4024,17 +4147,17 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="11"/>
-      <c r="B176" s="35"/>
+      <c r="A176" s="99"/>
+      <c r="B176" s="34"/>
       <c r="C176" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="9" t="s">
+      <c r="A177" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="B177" s="33" t="s">
+      <c r="B177" s="32" t="s">
         <v>266</v>
       </c>
       <c r="C177" s="8" t="s">
@@ -4042,17 +4165,17 @@
       </c>
     </row>
     <row r="178" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="9"/>
-      <c r="B178" s="33"/>
+      <c r="A178" s="100"/>
+      <c r="B178" s="32"/>
       <c r="C178" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="6" t="s">
+      <c r="A179" s="98" t="s">
         <v>372</v>
       </c>
-      <c r="B179" s="34" t="s">
+      <c r="B179" s="33" t="s">
         <v>267</v>
       </c>
       <c r="C179" s="8" t="s">
@@ -4060,17 +4183,17 @@
       </c>
     </row>
     <row r="180" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="11"/>
-      <c r="B180" s="35"/>
+      <c r="A180" s="99"/>
+      <c r="B180" s="34"/>
       <c r="C180" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" s="9" t="s">
+      <c r="A181" s="100" t="s">
         <v>373</v>
       </c>
-      <c r="B181" s="33" t="s">
+      <c r="B181" s="32" t="s">
         <v>268</v>
       </c>
       <c r="C181" s="8" t="s">
@@ -4078,17 +4201,17 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="9"/>
-      <c r="B182" s="33"/>
+      <c r="A182" s="100"/>
+      <c r="B182" s="32"/>
       <c r="C182" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="6" t="s">
+      <c r="A183" s="98" t="s">
         <v>374</v>
       </c>
-      <c r="B183" s="34" t="s">
+      <c r="B183" s="33" t="s">
         <v>269</v>
       </c>
       <c r="C183" s="8" t="s">
@@ -4096,17 +4219,17 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="11"/>
-      <c r="B184" s="35"/>
+      <c r="A184" s="99"/>
+      <c r="B184" s="34"/>
       <c r="C184" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="9" t="s">
+      <c r="A185" s="100" t="s">
         <v>375</v>
       </c>
-      <c r="B185" s="33" t="s">
+      <c r="B185" s="32" t="s">
         <v>270</v>
       </c>
       <c r="C185" s="8" t="s">
@@ -4114,17 +4237,17 @@
       </c>
     </row>
     <row r="186" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="9"/>
-      <c r="B186" s="33"/>
+      <c r="A186" s="100"/>
+      <c r="B186" s="32"/>
       <c r="C186" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="6" t="s">
+      <c r="A187" s="98" t="s">
         <v>379</v>
       </c>
-      <c r="B187" s="34" t="s">
+      <c r="B187" s="33" t="s">
         <v>271</v>
       </c>
       <c r="C187" s="8" t="s">
@@ -4132,17 +4255,17 @@
       </c>
     </row>
     <row r="188" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="11"/>
-      <c r="B188" s="35"/>
+      <c r="A188" s="99"/>
+      <c r="B188" s="34"/>
       <c r="C188" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" s="9" t="s">
+      <c r="A189" s="100" t="s">
         <v>377</v>
       </c>
-      <c r="B189" s="33" t="s">
+      <c r="B189" s="32" t="s">
         <v>272</v>
       </c>
       <c r="C189" s="8" t="s">
@@ -4150,17 +4273,17 @@
       </c>
     </row>
     <row r="190" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="9"/>
-      <c r="B190" s="33"/>
+      <c r="A190" s="100"/>
+      <c r="B190" s="32"/>
       <c r="C190" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="6" t="s">
+      <c r="A191" s="98" t="s">
         <v>376</v>
       </c>
-      <c r="B191" s="34" t="s">
+      <c r="B191" s="33" t="s">
         <v>273</v>
       </c>
       <c r="C191" s="8" t="s">
@@ -4168,17 +4291,17 @@
       </c>
     </row>
     <row r="192" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="11"/>
-      <c r="B192" s="35"/>
+      <c r="A192" s="99"/>
+      <c r="B192" s="34"/>
       <c r="C192" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="6" t="s">
+      <c r="A193" s="98" t="s">
         <v>378</v>
       </c>
-      <c r="B193" s="34" t="s">
+      <c r="B193" s="33" t="s">
         <v>274</v>
       </c>
       <c r="C193" s="8" t="s">
@@ -4186,17 +4309,17 @@
       </c>
     </row>
     <row r="194" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A194" s="11"/>
-      <c r="B194" s="35"/>
+      <c r="A194" s="99"/>
+      <c r="B194" s="34"/>
       <c r="C194" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="6" t="s">
+      <c r="A195" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="B195" s="34" t="s">
+      <c r="B195" s="33" t="s">
         <v>275</v>
       </c>
       <c r="C195" s="8" t="s">
@@ -4204,17 +4327,17 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="11"/>
-      <c r="B196" s="35"/>
+      <c r="A196" s="102"/>
+      <c r="B196" s="34"/>
       <c r="C196" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="6" t="s">
+      <c r="A197" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="B197" s="34" t="s">
+      <c r="B197" s="33" t="s">
         <v>276</v>
       </c>
       <c r="C197" s="8" t="s">
@@ -4222,17 +4345,17 @@
       </c>
     </row>
     <row r="198" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="11"/>
-      <c r="B198" s="35"/>
+      <c r="A198" s="102"/>
+      <c r="B198" s="34"/>
       <c r="C198" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="6" t="s">
+      <c r="A199" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="B199" s="34" t="s">
+      <c r="B199" s="33" t="s">
         <v>277</v>
       </c>
       <c r="C199" s="8" t="s">
@@ -4240,17 +4363,17 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="11"/>
-      <c r="B200" s="35"/>
+      <c r="A200" s="102"/>
+      <c r="B200" s="34"/>
       <c r="C200" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="9" t="s">
+      <c r="A201" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="B201" s="33" t="s">
+      <c r="B201" s="32" t="s">
         <v>278</v>
       </c>
       <c r="C201" s="10" t="s">
@@ -4258,17 +4381,17 @@
       </c>
     </row>
     <row r="202" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A202" s="9"/>
-      <c r="B202" s="33"/>
+      <c r="A202" s="103"/>
+      <c r="B202" s="32"/>
       <c r="C202" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="6" t="s">
+      <c r="A203" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="B203" s="34" t="s">
+      <c r="B203" s="33" t="s">
         <v>279</v>
       </c>
       <c r="C203" s="8" t="s">
@@ -4276,17 +4399,17 @@
       </c>
     </row>
     <row r="204" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="11"/>
-      <c r="B204" s="35"/>
+      <c r="A204" s="102"/>
+      <c r="B204" s="34"/>
       <c r="C204" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205" s="9" t="s">
+      <c r="A205" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="B205" s="33" t="s">
+      <c r="B205" s="32" t="s">
         <v>280</v>
       </c>
       <c r="C205" s="10" t="s">
@@ -4294,17 +4417,17 @@
       </c>
     </row>
     <row r="206" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A206" s="9"/>
-      <c r="B206" s="33"/>
+      <c r="A206" s="103"/>
+      <c r="B206" s="32"/>
       <c r="C206" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="6" t="s">
+      <c r="A207" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="B207" s="34" t="s">
+      <c r="B207" s="33" t="s">
         <v>281</v>
       </c>
       <c r="C207" s="8" t="s">
@@ -4312,17 +4435,17 @@
       </c>
     </row>
     <row r="208" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="11"/>
-      <c r="B208" s="35"/>
+      <c r="A208" s="102"/>
+      <c r="B208" s="34"/>
       <c r="C208" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209" s="9" t="s">
+      <c r="A209" s="103" t="s">
         <v>380</v>
       </c>
-      <c r="B209" s="33" t="s">
+      <c r="B209" s="32" t="s">
         <v>282</v>
       </c>
       <c r="C209" s="8" t="s">
@@ -4330,17 +4453,17 @@
       </c>
     </row>
     <row r="210" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A210" s="9"/>
-      <c r="B210" s="33"/>
+      <c r="A210" s="103"/>
+      <c r="B210" s="32"/>
       <c r="C210" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="6" t="s">
+      <c r="A211" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="B211" s="34" t="s">
+      <c r="B211" s="33" t="s">
         <v>283</v>
       </c>
       <c r="C211" s="8" t="s">
@@ -4348,17 +4471,17 @@
       </c>
     </row>
     <row r="212" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="11"/>
-      <c r="B212" s="35"/>
+      <c r="A212" s="102"/>
+      <c r="B212" s="34"/>
       <c r="C212" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="9" t="s">
+      <c r="A213" s="103" t="s">
         <v>382</v>
       </c>
-      <c r="B213" s="33" t="s">
+      <c r="B213" s="32" t="s">
         <v>284</v>
       </c>
       <c r="C213" s="8" t="s">
@@ -4366,17 +4489,17 @@
       </c>
     </row>
     <row r="214" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="9"/>
-      <c r="B214" s="33"/>
+      <c r="A214" s="103"/>
+      <c r="B214" s="32"/>
       <c r="C214" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A215" s="6" t="s">
+      <c r="A215" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="B215" s="34" t="s">
+      <c r="B215" s="33" t="s">
         <v>285</v>
       </c>
       <c r="C215" s="8" t="s">
@@ -4384,17 +4507,17 @@
       </c>
     </row>
     <row r="216" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A216" s="11"/>
-      <c r="B216" s="35"/>
+      <c r="A216" s="102"/>
+      <c r="B216" s="34"/>
       <c r="C216" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A217" s="9" t="s">
+      <c r="A217" s="103" t="s">
         <v>384</v>
       </c>
-      <c r="B217" s="33" t="s">
+      <c r="B217" s="32" t="s">
         <v>286</v>
       </c>
       <c r="C217" s="8" t="s">
@@ -4402,17 +4525,17 @@
       </c>
     </row>
     <row r="218" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="9"/>
-      <c r="B218" s="33"/>
+      <c r="A218" s="103"/>
+      <c r="B218" s="32"/>
       <c r="C218" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" s="6" t="s">
+      <c r="A219" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="B219" s="34" t="s">
+      <c r="B219" s="33" t="s">
         <v>287</v>
       </c>
       <c r="C219" s="8" t="s">
@@ -4420,17 +4543,17 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="11"/>
-      <c r="B220" s="35"/>
+      <c r="A220" s="102"/>
+      <c r="B220" s="34"/>
       <c r="C220" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A221" s="9" t="s">
+      <c r="A221" s="103" t="s">
         <v>386</v>
       </c>
-      <c r="B221" s="33" t="s">
+      <c r="B221" s="32" t="s">
         <v>288</v>
       </c>
       <c r="C221" s="8" t="s">
@@ -4438,17 +4561,17 @@
       </c>
     </row>
     <row r="222" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A222" s="9"/>
-      <c r="B222" s="33"/>
+      <c r="A222" s="103"/>
+      <c r="B222" s="32"/>
       <c r="C222" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A223" s="6" t="s">
+      <c r="A223" s="101" t="s">
         <v>387</v>
       </c>
-      <c r="B223" s="34" t="s">
+      <c r="B223" s="33" t="s">
         <v>289</v>
       </c>
       <c r="C223" s="8" t="s">
@@ -4456,17 +4579,17 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A224" s="11"/>
-      <c r="B224" s="35"/>
+      <c r="A224" s="102"/>
+      <c r="B224" s="34"/>
       <c r="C224" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A225" s="6" t="s">
+      <c r="A225" s="101" t="s">
         <v>388</v>
       </c>
-      <c r="B225" s="34" t="s">
+      <c r="B225" s="33" t="s">
         <v>290</v>
       </c>
       <c r="C225" s="8" t="s">
@@ -4474,8 +4597,8 @@
       </c>
     </row>
     <row r="226" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A226" s="11"/>
-      <c r="B226" s="35"/>
+      <c r="A226" s="102"/>
+      <c r="B226" s="34"/>
       <c r="C226" s="13" t="s">
         <v>54</v>
       </c>
@@ -4484,14 +4607,14 @@
       <c r="A227" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B227" s="36"/>
+      <c r="B227" s="35"/>
       <c r="C227" s="25"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="B228" s="34" t="s">
+      <c r="B228" s="33" t="s">
         <v>178</v>
       </c>
       <c r="C228" s="8" t="s">
@@ -4500,58 +4623,58 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="9"/>
-      <c r="B229" s="33"/>
+      <c r="B229" s="32"/>
       <c r="C229" s="10" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="9"/>
-      <c r="B230" s="33"/>
+      <c r="B230" s="32"/>
       <c r="C230" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="9"/>
-      <c r="B231" s="33"/>
+      <c r="B231" s="32"/>
       <c r="C231" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="9"/>
-      <c r="B232" s="33"/>
+      <c r="B232" s="32"/>
       <c r="C232" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="9"/>
-      <c r="B233" s="33"/>
+      <c r="B233" s="32"/>
       <c r="C233" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A234" s="11"/>
-      <c r="B234" s="35"/>
+      <c r="B234" s="34"/>
       <c r="C234" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A235" s="64" t="s">
+      <c r="A235" s="122" t="s">
         <v>89</v>
       </c>
-      <c r="B235" s="65"/>
-      <c r="C235" s="66"/>
+      <c r="B235" s="123"/>
+      <c r="C235" s="124"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="B236" s="34" t="s">
+      <c r="B236" s="33" t="s">
         <v>179</v>
       </c>
       <c r="C236" s="7" t="s">
@@ -4560,7 +4683,7 @@
     </row>
     <row r="237" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A237" s="11"/>
-      <c r="B237" s="35"/>
+      <c r="B237" s="34"/>
       <c r="C237" s="12" t="s">
         <v>54</v>
       </c>
@@ -4569,7 +4692,7 @@
       <c r="A238" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="B238" s="34" t="s">
+      <c r="B238" s="33" t="s">
         <v>180</v>
       </c>
       <c r="C238" s="7" t="s">
@@ -4578,7 +4701,7 @@
     </row>
     <row r="239" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A239" s="11"/>
-      <c r="B239" s="35"/>
+      <c r="B239" s="34"/>
       <c r="C239" s="12" t="s">
         <v>54</v>
       </c>
@@ -4587,7 +4710,7 @@
       <c r="A240" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="B240" s="34" t="s">
+      <c r="B240" s="33" t="s">
         <v>181</v>
       </c>
       <c r="C240" s="4" t="s">
@@ -4596,7 +4719,7 @@
     </row>
     <row r="241" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A241" s="11"/>
-      <c r="B241" s="35"/>
+      <c r="B241" s="34"/>
       <c r="C241" s="12" t="s">
         <v>54</v>
       </c>
@@ -4605,7 +4728,7 @@
       <c r="A242" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="B242" s="34" t="s">
+      <c r="B242" s="33" t="s">
         <v>182</v>
       </c>
       <c r="C242" s="7" t="s">
@@ -4614,7 +4737,7 @@
     </row>
     <row r="243" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A243" s="11"/>
-      <c r="B243" s="35"/>
+      <c r="B243" s="34"/>
       <c r="C243" s="12" t="s">
         <v>54</v>
       </c>
@@ -4623,7 +4746,7 @@
       <c r="A244" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B244" s="34" t="s">
+      <c r="B244" s="33" t="s">
         <v>183</v>
       </c>
       <c r="C244" s="7" t="s">
@@ -4632,7 +4755,7 @@
     </row>
     <row r="245" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A245" s="11"/>
-      <c r="B245" s="35"/>
+      <c r="B245" s="34"/>
       <c r="C245" s="12" t="s">
         <v>54</v>
       </c>
@@ -4641,7 +4764,7 @@
       <c r="A246" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="B246" s="34" t="s">
+      <c r="B246" s="33" t="s">
         <v>184</v>
       </c>
       <c r="C246" s="7" t="s">
@@ -4650,7 +4773,7 @@
     </row>
     <row r="247" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A247" s="11"/>
-      <c r="B247" s="35"/>
+      <c r="B247" s="34"/>
       <c r="C247" s="12" t="s">
         <v>54</v>
       </c>
@@ -4659,7 +4782,7 @@
       <c r="A248" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="B248" s="34" t="s">
+      <c r="B248" s="33" t="s">
         <v>185</v>
       </c>
       <c r="C248" s="7" t="s">
@@ -4668,7 +4791,7 @@
     </row>
     <row r="249" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A249" s="11"/>
-      <c r="B249" s="35"/>
+      <c r="B249" s="34"/>
       <c r="C249" s="12" t="s">
         <v>54</v>
       </c>
@@ -4677,7 +4800,7 @@
       <c r="A250" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="B250" s="34" t="s">
+      <c r="B250" s="33" t="s">
         <v>186</v>
       </c>
       <c r="C250" s="7" t="s">
@@ -4686,7 +4809,7 @@
     </row>
     <row r="251" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A251" s="11"/>
-      <c r="B251" s="35"/>
+      <c r="B251" s="34"/>
       <c r="C251" s="12" t="s">
         <v>54</v>
       </c>
@@ -4695,7 +4818,7 @@
       <c r="A252" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="B252" s="34" t="s">
+      <c r="B252" s="33" t="s">
         <v>187</v>
       </c>
       <c r="C252" s="7" t="s">
@@ -4704,7 +4827,7 @@
     </row>
     <row r="253" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A253" s="11"/>
-      <c r="B253" s="35"/>
+      <c r="B253" s="34"/>
       <c r="C253" s="12" t="s">
         <v>54</v>
       </c>
@@ -4713,7 +4836,7 @@
       <c r="A254" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="B254" s="34" t="s">
+      <c r="B254" s="33" t="s">
         <v>188</v>
       </c>
       <c r="C254" s="7" t="s">
@@ -4722,7 +4845,7 @@
     </row>
     <row r="255" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A255" s="11"/>
-      <c r="B255" s="35"/>
+      <c r="B255" s="34"/>
       <c r="C255" s="12" t="s">
         <v>54</v>
       </c>
@@ -4731,7 +4854,7 @@
       <c r="A256" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B256" s="34" t="s">
+      <c r="B256" s="33" t="s">
         <v>189</v>
       </c>
       <c r="C256" s="7" t="s">
@@ -4740,7 +4863,7 @@
     </row>
     <row r="257" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A257" s="11"/>
-      <c r="B257" s="35"/>
+      <c r="B257" s="34"/>
       <c r="C257" s="12" t="s">
         <v>54</v>
       </c>
@@ -4749,7 +4872,7 @@
       <c r="A258" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="B258" s="34" t="s">
+      <c r="B258" s="33" t="s">
         <v>190</v>
       </c>
       <c r="C258" s="7" t="s">
@@ -4758,7 +4881,7 @@
     </row>
     <row r="259" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A259" s="11"/>
-      <c r="B259" s="35"/>
+      <c r="B259" s="34"/>
       <c r="C259" s="12" t="s">
         <v>54</v>
       </c>
@@ -4767,7 +4890,7 @@
       <c r="A260" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="B260" s="32" t="s">
+      <c r="B260" s="31" t="s">
         <v>291</v>
       </c>
       <c r="C260" s="13"/>
@@ -4776,7 +4899,7 @@
       <c r="A261" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="B261" s="34" t="s">
+      <c r="B261" s="33" t="s">
         <v>292</v>
       </c>
       <c r="C261" s="8" t="s">
@@ -4785,7 +4908,7 @@
     </row>
     <row r="262" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A262" s="11"/>
-      <c r="B262" s="35"/>
+      <c r="B262" s="34"/>
       <c r="C262" s="13" t="s">
         <v>90</v>
       </c>
@@ -4794,7 +4917,7 @@
       <c r="A263" s="14" t="s">
         <v>404</v>
       </c>
-      <c r="B263" s="32" t="s">
+      <c r="B263" s="31" t="s">
         <v>293</v>
       </c>
       <c r="C263" s="21"/>
@@ -4803,7 +4926,7 @@
       <c r="A264" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="B264" s="34" t="s">
+      <c r="B264" s="33" t="s">
         <v>294</v>
       </c>
       <c r="C264" s="8" t="s">
@@ -4812,21 +4935,21 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="9"/>
-      <c r="B265" s="33"/>
+      <c r="B265" s="32"/>
       <c r="C265" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="9"/>
-      <c r="B266" s="33"/>
+      <c r="B266" s="32"/>
       <c r="C266" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A267" s="11"/>
-      <c r="B267" s="35"/>
+      <c r="B267" s="34"/>
       <c r="C267" s="13" t="s">
         <v>32</v>
       </c>
@@ -4835,7 +4958,7 @@
       <c r="A268" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="B268" s="34" t="s">
+      <c r="B268" s="33" t="s">
         <v>295</v>
       </c>
       <c r="C268" s="8" t="s">
@@ -4844,37 +4967,37 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="9"/>
-      <c r="B269" s="33"/>
+      <c r="B269" s="32"/>
       <c r="C269" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="9"/>
-      <c r="B270" s="33"/>
+      <c r="B270" s="32"/>
       <c r="C270" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="9"/>
-      <c r="B271" s="33"/>
+      <c r="B271" s="32"/>
       <c r="C271" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A272" s="11"/>
-      <c r="B272" s="35"/>
+      <c r="B272" s="34"/>
       <c r="C272" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A273" s="43" t="s">
+      <c r="A273" s="152" t="s">
         <v>407</v>
       </c>
-      <c r="B273" s="34" t="s">
+      <c r="B273" s="33" t="s">
         <v>296</v>
       </c>
       <c r="C273" s="8" t="s">
@@ -4882,15 +5005,15 @@
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A274" s="44"/>
-      <c r="B274" s="33"/>
+      <c r="A274" s="153"/>
+      <c r="B274" s="32"/>
       <c r="C274" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A275" s="11"/>
-      <c r="B275" s="35"/>
+      <c r="B275" s="34"/>
       <c r="C275" s="13" t="s">
         <v>100</v>
       </c>
@@ -4899,7 +5022,7 @@
       <c r="A276" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="B276" s="32" t="s">
+      <c r="B276" s="31" t="s">
         <v>297</v>
       </c>
       <c r="C276" s="21"/>
@@ -4908,7 +5031,7 @@
       <c r="A277" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="B277" s="34" t="s">
+      <c r="B277" s="33" t="s">
         <v>298</v>
       </c>
       <c r="C277" s="8" t="s">
@@ -4917,14 +5040,14 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="9"/>
-      <c r="B278" s="33"/>
+      <c r="B278" s="32"/>
       <c r="C278" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A279" s="11"/>
-      <c r="B279" s="35"/>
+      <c r="B279" s="34"/>
       <c r="C279" s="13" t="s">
         <v>102</v>
       </c>
@@ -4933,7 +5056,7 @@
       <c r="A280" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="B280" s="34" t="s">
+      <c r="B280" s="33" t="s">
         <v>299</v>
       </c>
       <c r="C280" s="8" t="s">
@@ -4942,7 +5065,7 @@
     </row>
     <row r="281" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A281" s="11"/>
-      <c r="B281" s="35"/>
+      <c r="B281" s="34"/>
       <c r="C281" s="13" t="s">
         <v>90</v>
       </c>
@@ -4951,7 +5074,7 @@
       <c r="A282" s="14" t="s">
         <v>404</v>
       </c>
-      <c r="B282" s="32" t="s">
+      <c r="B282" s="31" t="s">
         <v>300</v>
       </c>
       <c r="C282" s="21"/>
@@ -4960,7 +5083,7 @@
       <c r="A283" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="B283" s="34" t="s">
+      <c r="B283" s="33" t="s">
         <v>301</v>
       </c>
       <c r="C283" s="8" t="s">
@@ -4969,21 +5092,21 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="9"/>
-      <c r="B284" s="33"/>
+      <c r="B284" s="32"/>
       <c r="C284" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" s="9"/>
-      <c r="B285" s="33"/>
+      <c r="B285" s="32"/>
       <c r="C285" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="286" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A286" s="11"/>
-      <c r="B286" s="35"/>
+      <c r="B286" s="34"/>
       <c r="C286" s="13" t="s">
         <v>32</v>
       </c>
@@ -4992,7 +5115,7 @@
       <c r="A287" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="B287" s="34" t="s">
+      <c r="B287" s="33" t="s">
         <v>302</v>
       </c>
       <c r="C287" s="8" t="s">
@@ -5001,37 +5124,37 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" s="9"/>
-      <c r="B288" s="33"/>
+      <c r="B288" s="32"/>
       <c r="C288" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" s="9"/>
-      <c r="B289" s="33"/>
+      <c r="B289" s="32"/>
       <c r="C289" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" s="9"/>
-      <c r="B290" s="33"/>
+      <c r="B290" s="32"/>
       <c r="C290" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A291" s="11"/>
-      <c r="B291" s="35"/>
+      <c r="B291" s="34"/>
       <c r="C291" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A292" s="45" t="s">
+      <c r="A292" s="141" t="s">
         <v>407</v>
       </c>
-      <c r="B292" s="34" t="s">
+      <c r="B292" s="33" t="s">
         <v>303</v>
       </c>
       <c r="C292" s="8" t="s">
@@ -5039,15 +5162,15 @@
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A293" s="46"/>
-      <c r="B293" s="33"/>
+      <c r="A293" s="154"/>
+      <c r="B293" s="32"/>
       <c r="C293" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A294" s="47"/>
-      <c r="B294" s="35"/>
+      <c r="A294" s="142"/>
+      <c r="B294" s="34"/>
       <c r="C294" s="13" t="s">
         <v>100</v>
       </c>
@@ -5056,7 +5179,7 @@
       <c r="A295" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="B295" s="32" t="s">
+      <c r="B295" s="31" t="s">
         <v>304</v>
       </c>
       <c r="C295" s="21"/>
@@ -5065,7 +5188,7 @@
       <c r="A296" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="B296" s="34" t="s">
+      <c r="B296" s="33" t="s">
         <v>305</v>
       </c>
       <c r="C296" s="8" t="s">
@@ -5074,14 +5197,14 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" s="9"/>
-      <c r="B297" s="33"/>
+      <c r="B297" s="32"/>
       <c r="C297" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A298" s="11"/>
-      <c r="B298" s="35"/>
+      <c r="B298" s="34"/>
       <c r="C298" s="13" t="s">
         <v>102</v>
       </c>
@@ -5090,419 +5213,419 @@
       <c r="A299" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B299" s="36"/>
+      <c r="B299" s="35"/>
       <c r="C299" s="25"/>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A300" s="45" t="s">
+      <c r="A300" s="115" t="s">
         <v>411</v>
       </c>
-      <c r="B300" s="34" t="s">
+      <c r="B300" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="C300" s="8" t="s">
+      <c r="C300" s="57" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A301" s="47"/>
-      <c r="B301" s="35"/>
-      <c r="C301" s="13" t="s">
+      <c r="A301" s="116"/>
+      <c r="B301" s="61"/>
+      <c r="C301" s="58" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A302" s="6" t="s">
+      <c r="A302" s="53" t="s">
         <v>412</v>
       </c>
-      <c r="B302" s="34" t="s">
+      <c r="B302" s="60" t="s">
         <v>192</v>
       </c>
-      <c r="C302" s="21"/>
+      <c r="C302" s="59"/>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A303" s="45" t="s">
+      <c r="A303" s="117" t="s">
         <v>413</v>
       </c>
-      <c r="B303" s="34" t="s">
+      <c r="B303" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="C303" s="8" t="s">
+      <c r="C303" s="63" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A304" s="47"/>
-      <c r="B304" s="35"/>
-      <c r="C304" s="13" t="s">
+      <c r="A304" s="118"/>
+      <c r="B304" s="64"/>
+      <c r="C304" s="65" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A305" s="14" t="s">
+      <c r="A305" s="66" t="s">
         <v>414</v>
       </c>
-      <c r="B305" s="32" t="s">
+      <c r="B305" s="67" t="s">
         <v>194</v>
       </c>
-      <c r="C305" s="21"/>
+      <c r="C305" s="68"/>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A306" s="45" t="s">
+      <c r="A306" s="115" t="s">
         <v>235</v>
       </c>
-      <c r="B306" s="34" t="s">
+      <c r="B306" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="C306" s="8" t="s">
+      <c r="C306" s="57" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A307" s="47"/>
-      <c r="B307" s="35"/>
-      <c r="C307" s="13" t="s">
+      <c r="A307" s="116"/>
+      <c r="B307" s="61"/>
+      <c r="C307" s="58" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A308" s="6" t="s">
+      <c r="A308" s="53" t="s">
         <v>415</v>
       </c>
-      <c r="B308" s="34" t="s">
+      <c r="B308" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="C308" s="21"/>
+      <c r="C308" s="59"/>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A309" s="45" t="s">
+      <c r="A309" s="117" t="s">
         <v>236</v>
       </c>
-      <c r="B309" s="34" t="s">
+      <c r="B309" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="C309" s="8" t="s">
+      <c r="C309" s="63" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A310" s="47"/>
-      <c r="B310" s="35"/>
-      <c r="C310" s="13" t="s">
+      <c r="A310" s="118"/>
+      <c r="B310" s="64"/>
+      <c r="C310" s="65" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A311" s="14" t="s">
+      <c r="A311" s="66" t="s">
         <v>416</v>
       </c>
-      <c r="B311" s="32" t="s">
+      <c r="B311" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C311" s="8"/>
+      <c r="C311" s="63"/>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A312" s="67" t="s">
+      <c r="A312" s="37" t="s">
         <v>417</v>
       </c>
-      <c r="B312" s="68" t="s">
+      <c r="B312" s="125" t="s">
         <v>199</v>
       </c>
-      <c r="C312" s="69" t="s">
+      <c r="C312" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A313" s="70"/>
-      <c r="B313" s="71"/>
-      <c r="C313" s="72" t="s">
+      <c r="A313" s="39"/>
+      <c r="B313" s="126"/>
+      <c r="C313" s="40" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A314" s="73"/>
-      <c r="B314" s="74"/>
-      <c r="C314" s="75" t="s">
+      <c r="A314" s="41"/>
+      <c r="B314" s="127"/>
+      <c r="C314" s="42" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A315" s="76" t="s">
+      <c r="A315" s="43" t="s">
         <v>418</v>
       </c>
-      <c r="B315" s="77" t="s">
+      <c r="B315" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="C315" s="78"/>
+      <c r="C315" s="69"/>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A316" s="83" t="s">
+      <c r="A316" s="45" t="s">
         <v>419</v>
       </c>
-      <c r="B316" s="84" t="s">
+      <c r="B316" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="C316" s="85" t="s">
+      <c r="C316" s="46" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A317" s="86"/>
-      <c r="B317" s="87"/>
-      <c r="C317" s="88" t="s">
+      <c r="A317" s="47"/>
+      <c r="B317" s="129"/>
+      <c r="C317" s="48" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A318" s="89"/>
-      <c r="B318" s="90"/>
-      <c r="C318" s="91" t="s">
+      <c r="A318" s="49"/>
+      <c r="B318" s="130"/>
+      <c r="C318" s="50" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A319" s="92" t="s">
+      <c r="A319" s="51" t="s">
         <v>420</v>
       </c>
-      <c r="B319" s="93" t="s">
+      <c r="B319" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="C319" s="94"/>
+      <c r="C319" s="52"/>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A320" s="95" t="s">
+      <c r="A320" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="B320" s="96" t="s">
+      <c r="B320" s="128" t="s">
         <v>203</v>
       </c>
-      <c r="C320" s="97" t="s">
+      <c r="C320" s="46" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A321" s="98"/>
-      <c r="B321" s="99"/>
-      <c r="C321" s="100" t="s">
+      <c r="A321" s="47"/>
+      <c r="B321" s="129"/>
+      <c r="C321" s="48" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A322" s="101"/>
-      <c r="B322" s="102"/>
-      <c r="C322" s="103" t="s">
+      <c r="A322" s="49"/>
+      <c r="B322" s="130"/>
+      <c r="C322" s="50" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A323" s="104" t="s">
+      <c r="A323" s="51" t="s">
         <v>421</v>
       </c>
-      <c r="B323" s="105" t="s">
+      <c r="B323" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="C323" s="106"/>
+      <c r="C323" s="52"/>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A324" s="107" t="s">
+      <c r="A324" s="110" t="s">
         <v>422</v>
       </c>
-      <c r="B324" s="108" t="s">
+      <c r="B324" s="131" t="s">
         <v>205</v>
       </c>
-      <c r="C324" s="109" t="s">
+      <c r="C324" s="80" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A325" s="110"/>
-      <c r="B325" s="111"/>
-      <c r="C325" s="112" t="s">
+      <c r="A325" s="111"/>
+      <c r="B325" s="132"/>
+      <c r="C325" s="81" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A326" s="113"/>
-      <c r="B326" s="114"/>
-      <c r="C326" s="115" t="s">
+      <c r="A326" s="112"/>
+      <c r="B326" s="133"/>
+      <c r="C326" s="82" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A327" s="116" t="s">
+      <c r="A327" s="83" t="s">
         <v>423</v>
       </c>
-      <c r="B327" s="117" t="s">
+      <c r="B327" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="C327" s="118"/>
+      <c r="C327" s="84"/>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A328" s="67" t="s">
+      <c r="A328" s="37" t="s">
         <v>425</v>
       </c>
-      <c r="B328" s="79" t="s">
+      <c r="B328" s="125" t="s">
         <v>207</v>
       </c>
-      <c r="C328" s="69" t="s">
+      <c r="C328" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A329" s="70"/>
-      <c r="B329" s="80"/>
-      <c r="C329" s="72" t="s">
+      <c r="A329" s="39"/>
+      <c r="B329" s="126"/>
+      <c r="C329" s="40" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A330" s="73"/>
-      <c r="B330" s="81"/>
-      <c r="C330" s="75" t="s">
+      <c r="A330" s="41"/>
+      <c r="B330" s="127"/>
+      <c r="C330" s="42" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="331" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A331" s="76" t="s">
+      <c r="A331" s="43" t="s">
         <v>424</v>
       </c>
-      <c r="B331" s="77" t="s">
+      <c r="B331" s="71" t="s">
         <v>208</v>
       </c>
-      <c r="C331" s="82"/>
+      <c r="C331" s="44"/>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A332" s="83" t="s">
+      <c r="A332" s="72" t="s">
         <v>426</v>
       </c>
-      <c r="B332" s="84" t="s">
+      <c r="B332" s="144" t="s">
         <v>209</v>
       </c>
-      <c r="C332" s="85" t="s">
+      <c r="C332" s="73" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A333" s="86"/>
-      <c r="B333" s="87"/>
-      <c r="C333" s="88" t="s">
+      <c r="A333" s="74"/>
+      <c r="B333" s="145"/>
+      <c r="C333" s="75" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A334" s="89"/>
-      <c r="B334" s="90"/>
-      <c r="C334" s="91" t="s">
+      <c r="A334" s="76"/>
+      <c r="B334" s="146"/>
+      <c r="C334" s="77" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="335" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A335" s="92" t="s">
+      <c r="A335" s="78" t="s">
         <v>427</v>
       </c>
-      <c r="B335" s="93" t="s">
+      <c r="B335" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="C335" s="94"/>
+      <c r="C335" s="79"/>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A336" s="95" t="s">
+      <c r="A336" s="72" t="s">
         <v>428</v>
       </c>
-      <c r="B336" s="96" t="s">
+      <c r="B336" s="144" t="s">
         <v>210</v>
       </c>
-      <c r="C336" s="97" t="s">
+      <c r="C336" s="73" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A337" s="98"/>
-      <c r="B337" s="99"/>
-      <c r="C337" s="100" t="s">
+      <c r="A337" s="74"/>
+      <c r="B337" s="145"/>
+      <c r="C337" s="75" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A338" s="101"/>
-      <c r="B338" s="102"/>
-      <c r="C338" s="103" t="s">
+      <c r="A338" s="76"/>
+      <c r="B338" s="146"/>
+      <c r="C338" s="77" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A339" s="104" t="s">
+      <c r="A339" s="78" t="s">
         <v>429</v>
       </c>
-      <c r="B339" s="105" t="s">
+      <c r="B339" s="85" t="s">
         <v>211</v>
       </c>
-      <c r="C339" s="106"/>
+      <c r="C339" s="79"/>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A340" s="107" t="s">
+      <c r="A340" s="110" t="s">
         <v>430</v>
       </c>
-      <c r="B340" s="108" t="s">
+      <c r="B340" s="131" t="s">
         <v>212</v>
       </c>
-      <c r="C340" s="109" t="s">
+      <c r="C340" s="80" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A341" s="110"/>
-      <c r="B341" s="111"/>
-      <c r="C341" s="112" t="s">
+      <c r="A341" s="111"/>
+      <c r="B341" s="132"/>
+      <c r="C341" s="81" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A342" s="113"/>
-      <c r="B342" s="114"/>
-      <c r="C342" s="115" t="s">
+      <c r="A342" s="112"/>
+      <c r="B342" s="133"/>
+      <c r="C342" s="82" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A343" s="116" t="s">
+      <c r="A343" s="83" t="s">
         <v>431</v>
       </c>
-      <c r="B343" s="117" t="s">
+      <c r="B343" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="C343" s="118"/>
+      <c r="C343" s="84"/>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A344" s="119" t="s">
+      <c r="A344" s="87" t="s">
         <v>432</v>
       </c>
-      <c r="B344" s="120" t="s">
+      <c r="B344" s="147" t="s">
         <v>214</v>
       </c>
-      <c r="C344" s="121" t="s">
+      <c r="C344" s="55" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A345" s="122"/>
-      <c r="B345" s="123"/>
-      <c r="C345" s="124" t="s">
+      <c r="A345" s="88"/>
+      <c r="B345" s="148"/>
+      <c r="C345" s="56" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A346" s="125"/>
-      <c r="B346" s="126"/>
-      <c r="C346" s="127" t="s">
+      <c r="A346" s="89"/>
+      <c r="B346" s="149"/>
+      <c r="C346" s="54" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A347" s="6" t="s">
+      <c r="A347" s="87" t="s">
         <v>433</v>
       </c>
-      <c r="B347" s="34" t="s">
+      <c r="B347" s="33" t="s">
         <v>215</v>
       </c>
       <c r="C347" s="8" t="s">
@@ -5510,24 +5633,24 @@
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A348" s="9"/>
-      <c r="B348" s="33"/>
+      <c r="A348" s="88"/>
+      <c r="B348" s="32"/>
       <c r="C348" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A349" s="11"/>
-      <c r="B349" s="35"/>
+      <c r="A349" s="89"/>
+      <c r="B349" s="34"/>
       <c r="C349" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A350" s="6" t="s">
+      <c r="A350" s="87" t="s">
         <v>434</v>
       </c>
-      <c r="B350" s="34" t="s">
+      <c r="B350" s="33" t="s">
         <v>216</v>
       </c>
       <c r="C350" s="8" t="s">
@@ -5535,24 +5658,24 @@
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A351" s="9"/>
-      <c r="B351" s="33"/>
+      <c r="A351" s="88"/>
+      <c r="B351" s="32"/>
       <c r="C351" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="352" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A352" s="11"/>
-      <c r="B352" s="35"/>
+      <c r="A352" s="89"/>
+      <c r="B352" s="34"/>
       <c r="C352" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A353" s="6" t="s">
+      <c r="A353" s="87" t="s">
         <v>435</v>
       </c>
-      <c r="B353" s="34" t="s">
+      <c r="B353" s="33" t="s">
         <v>217</v>
       </c>
       <c r="C353" s="8" t="s">
@@ -5560,24 +5683,24 @@
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A354" s="9"/>
-      <c r="B354" s="33"/>
+      <c r="A354" s="88"/>
+      <c r="B354" s="32"/>
       <c r="C354" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="355" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A355" s="11"/>
-      <c r="B355" s="35"/>
+      <c r="A355" s="89"/>
+      <c r="B355" s="34"/>
       <c r="C355" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A356" s="6" t="s">
+      <c r="A356" s="87" t="s">
         <v>436</v>
       </c>
-      <c r="B356" s="34" t="s">
+      <c r="B356" s="33" t="s">
         <v>218</v>
       </c>
       <c r="C356" s="8" t="s">
@@ -5585,24 +5708,24 @@
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A357" s="9"/>
-      <c r="B357" s="33"/>
+      <c r="A357" s="88"/>
+      <c r="B357" s="32"/>
       <c r="C357" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A358" s="11"/>
-      <c r="B358" s="35"/>
+      <c r="A358" s="89"/>
+      <c r="B358" s="34"/>
       <c r="C358" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A359" s="6" t="s">
+      <c r="A359" s="87" t="s">
         <v>437</v>
       </c>
-      <c r="B359" s="34" t="s">
+      <c r="B359" s="33" t="s">
         <v>219</v>
       </c>
       <c r="C359" s="8" t="s">
@@ -5610,24 +5733,24 @@
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A360" s="9"/>
-      <c r="B360" s="33"/>
+      <c r="A360" s="88"/>
+      <c r="B360" s="32"/>
       <c r="C360" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A361" s="11"/>
-      <c r="B361" s="35"/>
+      <c r="A361" s="89"/>
+      <c r="B361" s="34"/>
       <c r="C361" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A362" s="6" t="s">
+      <c r="A362" s="87" t="s">
         <v>438</v>
       </c>
-      <c r="B362" s="34" t="s">
+      <c r="B362" s="33" t="s">
         <v>220</v>
       </c>
       <c r="C362" s="8" t="s">
@@ -5635,24 +5758,24 @@
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A363" s="9"/>
-      <c r="B363" s="33"/>
+      <c r="A363" s="88"/>
+      <c r="B363" s="32"/>
       <c r="C363" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="364" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A364" s="11"/>
-      <c r="B364" s="35"/>
+      <c r="A364" s="89"/>
+      <c r="B364" s="34"/>
       <c r="C364" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A365" s="6" t="s">
+      <c r="A365" s="87" t="s">
         <v>439</v>
       </c>
-      <c r="B365" s="34" t="s">
+      <c r="B365" s="33" t="s">
         <v>221</v>
       </c>
       <c r="C365" s="8" t="s">
@@ -5660,24 +5783,24 @@
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A366" s="9"/>
-      <c r="B366" s="33"/>
+      <c r="A366" s="88"/>
+      <c r="B366" s="32"/>
       <c r="C366" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="367" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A367" s="11"/>
-      <c r="B367" s="35"/>
+      <c r="A367" s="89"/>
+      <c r="B367" s="34"/>
       <c r="C367" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A368" s="6" t="s">
+      <c r="A368" s="87" t="s">
         <v>440</v>
       </c>
-      <c r="B368" s="34" t="s">
+      <c r="B368" s="33" t="s">
         <v>222</v>
       </c>
       <c r="C368" s="8" t="s">
@@ -5685,24 +5808,24 @@
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A369" s="9"/>
-      <c r="B369" s="33"/>
+      <c r="A369" s="88"/>
+      <c r="B369" s="32"/>
       <c r="C369" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="370" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A370" s="11"/>
-      <c r="B370" s="35"/>
+      <c r="A370" s="89"/>
+      <c r="B370" s="34"/>
       <c r="C370" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A371" s="6" t="s">
+      <c r="A371" s="87" t="s">
         <v>441</v>
       </c>
-      <c r="B371" s="34" t="s">
+      <c r="B371" s="33" t="s">
         <v>223</v>
       </c>
       <c r="C371" s="8" t="s">
@@ -5710,15 +5833,15 @@
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A372" s="9"/>
-      <c r="B372" s="33"/>
+      <c r="A372" s="88"/>
+      <c r="B372" s="32"/>
       <c r="C372" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A373" s="11"/>
-      <c r="B373" s="35"/>
+      <c r="A373" s="89"/>
+      <c r="B373" s="34"/>
       <c r="C373" s="13" t="s">
         <v>132</v>
       </c>
@@ -5727,7 +5850,7 @@
       <c r="A374" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="B374" s="34" t="s">
+      <c r="B374" s="33" t="s">
         <v>224</v>
       </c>
       <c r="C374" s="8" t="s">
@@ -5736,49 +5859,49 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" s="9"/>
-      <c r="B375" s="33"/>
+      <c r="B375" s="32"/>
       <c r="C375" s="10" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" s="9"/>
-      <c r="B376" s="33"/>
+      <c r="B376" s="32"/>
       <c r="C376" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" s="9"/>
-      <c r="B377" s="33"/>
+      <c r="B377" s="32"/>
       <c r="C377" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" s="9"/>
-      <c r="B378" s="33"/>
+      <c r="B378" s="32"/>
       <c r="C378" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" s="9"/>
-      <c r="B379" s="33"/>
+      <c r="B379" s="32"/>
       <c r="C379" s="10" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" s="9"/>
-      <c r="B380" s="33"/>
+      <c r="B380" s="32"/>
       <c r="C380" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="381" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A381" s="11"/>
-      <c r="B381" s="35"/>
+      <c r="B381" s="34"/>
       <c r="C381" s="13" t="s">
         <v>126</v>
       </c>
@@ -5787,7 +5910,7 @@
       <c r="A382" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="B382" s="33" t="s">
+      <c r="B382" s="32" t="s">
         <v>225</v>
       </c>
       <c r="C382" s="10"/>
@@ -5796,7 +5919,7 @@
       <c r="A383" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="B383" s="34" t="s">
+      <c r="B383" s="33" t="s">
         <v>226</v>
       </c>
       <c r="C383" s="8" t="s">
@@ -5805,28 +5928,28 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" s="9"/>
-      <c r="B384" s="33"/>
+      <c r="B384" s="32"/>
       <c r="C384" s="10" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="9"/>
-      <c r="B385" s="33"/>
+      <c r="B385" s="32"/>
       <c r="C385" s="10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" s="9"/>
-      <c r="B386" s="33"/>
+      <c r="B386" s="32"/>
       <c r="C386" s="10" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="387" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A387" s="9"/>
-      <c r="B387" s="33"/>
+      <c r="B387" s="32"/>
       <c r="C387" s="10" t="s">
         <v>307</v>
       </c>
@@ -5835,23 +5958,23 @@
       <c r="A388" s="22" t="s">
         <v>447</v>
       </c>
-      <c r="B388" s="36"/>
+      <c r="B388" s="35"/>
       <c r="C388" s="25"/>
     </row>
     <row r="389" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A389" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B389" s="32" t="s">
+      <c r="B389" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="C389" s="30"/>
+      <c r="C389" s="29"/>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A390" s="38" t="s">
+      <c r="A390" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="B390" s="57" t="s">
+      <c r="B390" s="107" t="s">
         <v>229</v>
       </c>
       <c r="C390" s="7" t="s">
@@ -5859,70 +5982,83 @@
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A391" s="39"/>
-      <c r="B391" s="58"/>
+      <c r="A391" s="105"/>
+      <c r="B391" s="108"/>
       <c r="C391" s="4" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A392" s="39"/>
-      <c r="B392" s="58"/>
+      <c r="A392" s="105"/>
+      <c r="B392" s="108"/>
       <c r="C392" s="4" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A393" s="39"/>
-      <c r="B393" s="58"/>
+      <c r="A393" s="105"/>
+      <c r="B393" s="108"/>
       <c r="C393" s="4" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A394" s="39"/>
-      <c r="B394" s="58"/>
+      <c r="A394" s="105"/>
+      <c r="B394" s="108"/>
       <c r="C394" s="4" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A395" s="39"/>
-      <c r="B395" s="58"/>
+      <c r="A395" s="105"/>
+      <c r="B395" s="108"/>
       <c r="C395" s="4" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A396" s="39"/>
-      <c r="B396" s="58"/>
+      <c r="A396" s="105"/>
+      <c r="B396" s="108"/>
       <c r="C396" s="4" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A397" s="39"/>
-      <c r="B397" s="58"/>
+      <c r="A397" s="105"/>
+      <c r="B397" s="108"/>
       <c r="C397" s="4" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A398" s="39"/>
-      <c r="B398" s="58"/>
+      <c r="A398" s="105"/>
+      <c r="B398" s="108"/>
       <c r="C398" s="4" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="399" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A399" s="40"/>
-      <c r="B399" s="59"/>
+      <c r="A399" s="106"/>
+      <c r="B399" s="109"/>
       <c r="C399" s="12" t="s">
         <v>457</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="29">
+    <mergeCell ref="B332:B334"/>
+    <mergeCell ref="B336:B338"/>
+    <mergeCell ref="B340:B342"/>
+    <mergeCell ref="B344:B346"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A273:A274"/>
+    <mergeCell ref="A292:A294"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="B49:B56"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="A390:A399"/>
     <mergeCell ref="B390:B399"/>
     <mergeCell ref="A340:A342"/>
@@ -5934,15 +6070,11 @@
     <mergeCell ref="A110:A112"/>
     <mergeCell ref="A235:C235"/>
     <mergeCell ref="A324:A326"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A273:A274"/>
-    <mergeCell ref="A292:A294"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="B49:B56"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B312:B314"/>
+    <mergeCell ref="B316:B318"/>
+    <mergeCell ref="B320:B322"/>
+    <mergeCell ref="B324:B326"/>
+    <mergeCell ref="B328:B330"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>